<commit_message>
progress, rearranged files for abgabe
</commit_message>
<xml_diff>
--- a/Thesis/Fragestellungen.xlsx
+++ b/Thesis/Fragestellungen.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4500" yWindow="0" windowWidth="19200" windowHeight="11580" activeTab="1"/>
+    <workbookView xWindow="6000" yWindow="0" windowWidth="19200" windowHeight="11580" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Fragestellungen" sheetId="1" r:id="rId1"/>
@@ -1161,29 +1161,23 @@
   </cellStyles>
   <dxfs count="26">
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -1203,23 +1197,12 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -1546,6 +1529,23 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -1726,7 +1726,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -1783,6 +1785,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="l"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1989,7 +1992,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -2008,7 +2013,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -2027,7 +2034,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -2069,6 +2078,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -2110,7 +2120,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -2141,7 +2153,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -2293,6 +2307,7 @@
         <c:idx val="4"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2478,7 +2493,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -2538,6 +2555,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="l"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2708,7 +2726,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -2765,6 +2785,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="l"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2950,7 +2971,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -3010,6 +3033,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="l"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3180,7 +3204,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -3237,6 +3263,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="l"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3422,7 +3449,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -3482,6 +3511,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="l"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3677,7 +3707,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -3696,7 +3728,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -3715,7 +3749,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -3734,7 +3770,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -3753,7 +3791,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -3772,7 +3812,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -3905,6 +3947,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="l"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4117,7 +4160,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4136,7 +4181,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4155,7 +4202,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4174,7 +4223,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4193,7 +4244,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4212,7 +4265,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4231,7 +4286,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -4380,6 +4437,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="l"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4546,7 +4604,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4565,7 +4625,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4603,6 +4665,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -4660,7 +4723,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -4737,6 +4802,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="l"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10731,27 +10797,27 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle2" displayName="Tabelle2" ref="A2:O238" totalsRowShown="0" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle2" displayName="Tabelle2" ref="A2:O238" totalsRowShown="0" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16" totalsRowBorderDxfId="15">
   <autoFilter ref="A2:O238"/>
   <sortState ref="A3:O238">
     <sortCondition descending="1" ref="H2:H238"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" name="Spalte1" dataDxfId="16"/>
-    <tableColumn id="2" name="Full" dataDxfId="15"/>
-    <tableColumn id="4" name="Tech" dataDxfId="14"/>
-    <tableColumn id="5" name="Full2" dataDxfId="13"/>
-    <tableColumn id="7" name="Tech4" dataDxfId="12"/>
-    <tableColumn id="8" name="Full5" dataDxfId="11"/>
-    <tableColumn id="10" name="Tech7" dataDxfId="10"/>
-    <tableColumn id="11" name="Full8" dataDxfId="9"/>
-    <tableColumn id="13" name="Tech10" dataDxfId="8"/>
-    <tableColumn id="14" name="Mehr-deutig" dataDxfId="7"/>
-    <tableColumn id="20" name="Je eine Bedeutung" dataDxfId="2"/>
-    <tableColumn id="15" name="Full11" dataDxfId="6"/>
-    <tableColumn id="17" name="Tech13" dataDxfId="5"/>
-    <tableColumn id="18" name="Full14" dataDxfId="4"/>
-    <tableColumn id="19" name="Tech15" dataDxfId="3"/>
+    <tableColumn id="1" name="Spalte1" dataDxfId="14"/>
+    <tableColumn id="2" name="Full" dataDxfId="13"/>
+    <tableColumn id="4" name="Tech" dataDxfId="12"/>
+    <tableColumn id="5" name="Full2" dataDxfId="11"/>
+    <tableColumn id="7" name="Tech4" dataDxfId="10"/>
+    <tableColumn id="8" name="Full5" dataDxfId="9"/>
+    <tableColumn id="10" name="Tech7" dataDxfId="8"/>
+    <tableColumn id="11" name="Full8" dataDxfId="7"/>
+    <tableColumn id="13" name="Tech10" dataDxfId="6"/>
+    <tableColumn id="14" name="Mehr-deutig" dataDxfId="5"/>
+    <tableColumn id="20" name="Je eine Bedeutung" dataDxfId="4"/>
+    <tableColumn id="15" name="Full11" dataDxfId="3"/>
+    <tableColumn id="17" name="Tech13" dataDxfId="2"/>
+    <tableColumn id="18" name="Full14" dataDxfId="1"/>
+    <tableColumn id="19" name="Tech15" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -11147,7 +11213,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O251"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -20670,10 +20736,10 @@
     <mergeCell ref="J1:M1"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:G238">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="2" operator="equal">
       <formula>"-"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20689,7 +20755,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AF27" sqref="AF27"/>
     </sheetView>
   </sheetViews>

</xml_diff>